<commit_message>
cleanup and add venhts chapter draft
</commit_message>
<xml_diff>
--- a/user_guide/data/venhts_tracking.xlsx
+++ b/user_guide/data/venhts_tracking.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitclones\VisionEval-Docs\user_guide\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AF7BF5-1BB7-4734-9191-9FC1B2F172A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D782FB4-8A68-4652-821E-21757C25E649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="45" windowWidth="20190" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="30" windowWidth="23835" windowHeight="14835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="71">
   <si>
     <t>Module</t>
   </si>
@@ -583,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:E41"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,4 +1062,512 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DE9DB0-1809-4DB0-8929-4188533DD257}">
+  <dimension ref="B1:E47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>